<commit_message>
user guide structure fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Wintage.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Wintage.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Downloads\SSS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\Stability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA38297-9205-4550-B406-2FD6A59C7929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E70EBC5-F47E-4332-AD75-02A042AA8E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Windage " sheetId="1" r:id="rId1"/>
-    <sheet name="Horizontal surf" sheetId="2" r:id="rId2"/>
+    <sheet name="Windage X" sheetId="3" r:id="rId2"/>
+    <sheet name="Horizontal surf" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>d [m]</t>
   </si>
@@ -119,6 +120,36 @@
   </si>
   <si>
     <t>Crane fore</t>
+  </si>
+  <si>
+    <t>Выхлопная труба</t>
+  </si>
+  <si>
+    <t>Рубка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кран кормовой </t>
+  </si>
+  <si>
+    <t>Кран носовой</t>
+  </si>
+  <si>
+    <t>Area [m2]</t>
+  </si>
+  <si>
+    <t>Крышки и комингс кормового трюма</t>
+  </si>
+  <si>
+    <t>Крышки и комингс носового трюма</t>
+  </si>
+  <si>
+    <t>Ют</t>
+  </si>
+  <si>
+    <t>Бак</t>
+  </si>
+  <si>
+    <t>Надводный борт (выше 2,001)</t>
   </si>
 </sst>
 </file>
@@ -1214,10 +1245,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E36415-DD44-4569-AFFE-7A106D5E9833}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="11" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>

</xml_diff>